<commit_message>
Now includes U grades in output
</commit_message>
<xml_diff>
--- a/School1 Results.xlsx
+++ b/School1 Results.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3668B3E-B31B-47A8-9511-C48613ADF5E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>UPN</t>
   </si>
@@ -41,12 +42,18 @@
   </si>
   <si>
     <t>Surname 1</t>
+  </si>
+  <si>
+    <t>6018131X</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -172,6 +179,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -207,6 +231,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -382,25 +423,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.86328125" customWidth="1"/>
+    <col min="2" max="2" width="22.3984375" customWidth="1"/>
+    <col min="3" max="3" width="21.3984375" customWidth="1"/>
+    <col min="4" max="4" width="22.59765625" customWidth="1"/>
+    <col min="5" max="5" width="18.59765625" customWidth="1"/>
+    <col min="6" max="6" width="33.59765625" customWidth="1"/>
+    <col min="7" max="7" width="26.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -423,7 +464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -446,7 +487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -469,7 +510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -492,7 +533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -515,7 +556,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -536,6 +577,29 @@
       </c>
       <c r="G6">
         <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1">
+        <v>43647</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>